<commit_message>
ss: update cov forms
</commit_message>
<xml_diff>
--- a/Coverage Survey/South Sudan/ss_oncho_cov_2_202309_couv.xlsx
+++ b/Coverage Survey/South Sudan/ss_oncho_cov_2_202309_couv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\Coverage Survey\South Sudan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483B615B-0390-40B9-8CB5-54AE1A4EF060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5757995-73C3-4F59-9FFA-3653AF4BF732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>bf_oncho_cov_2_202309_couverture</t>
   </si>
   <si>
-    <t>(Sept 2023) BFA Cov ONCHO - 2.Formulaire Couverture</t>
-  </si>
-  <si>
     <t>Recorder ID</t>
   </si>
   <si>
@@ -971,6 +968,9 @@
   </si>
   <si>
     <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_swallow_ivm} = 'Yes'</t>
+  </si>
+  <si>
+    <t>(Sept 2023) SSD Cov ONCHO - 2.Formulaire Couverture</t>
   </si>
 </sst>
 </file>
@@ -1382,11 +1382,11 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1410,10 +1410,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1422,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -1442,22 +1442,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1465,10 +1465,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
@@ -1480,10 +1480,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
@@ -1495,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
@@ -1510,10 +1510,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
@@ -1522,23 +1522,23 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
         <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1546,30 +1546,30 @@
         <v>9</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
@@ -1578,16 +1578,16 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>16</v>
@@ -1596,18 +1596,18 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -1618,17 +1618,17 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1637,21 +1637,21 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>16</v>
@@ -1662,79 +1662,79 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>310</v>
-      </c>
       <c r="H14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1742,109 +1742,109 @@
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1852,81 +1852,81 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L27" s="13"/>
     </row>
@@ -1935,76 +1935,76 @@
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L31" s="13"/>
     </row>
@@ -2013,72 +2013,72 @@
         <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>242</v>
-      </c>
       <c r="C34" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
@@ -2086,60 +2086,60 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2147,71 +2147,71 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>261</v>
-      </c>
       <c r="C42" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2219,17 +2219,17 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2237,33 +2237,33 @@
         <v>9</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="10"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
@@ -2271,78 +2271,78 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2350,71 +2350,71 @@
         <v>9</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2422,19 +2422,19 @@
         <v>9</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2442,35 +2442,35 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
@@ -2478,110 +2478,110 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2593,13 +2593,13 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -2651,7 +2651,7 @@
   </sheetPr>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
@@ -2671,770 +2671,770 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" t="s">
         <v>124</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
         <v>143</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C48" t="s">
         <v>215</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C48" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C52" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C55" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C56" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C57" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C61" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C62" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C68" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C69" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -3478,7 +3478,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>311</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
ss: update form 2
</commit_message>
<xml_diff>
--- a/Coverage Survey/South Sudan/ss_oncho_cov_2_202309_couv.xlsx
+++ b/Coverage Survey/South Sudan/ss_oncho_cov_2_202309_couv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\Coverage Survey\South Sudan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5757995-73C3-4F59-9FFA-3653AF4BF732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0D7012-4190-40B6-8CEA-688E9F6E1E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="322">
   <si>
     <t>type</t>
   </si>
@@ -115,9 +115,6 @@
     <t>27. Notes</t>
   </si>
   <si>
-    <t>bf_oncho_cov_2_202309_couverture</t>
-  </si>
-  <si>
     <t>Recorder ID</t>
   </si>
   <si>
@@ -481,9 +478,6 @@
     <t>Someone on behalf as underage</t>
   </si>
   <si>
-    <t>p_responding</t>
-  </si>
-  <si>
     <t>Do not know</t>
   </si>
   <si>
@@ -529,9 +523,6 @@
     <t>9. If woman of child-bearing age are they pregnant or breastfeeding at present?</t>
   </si>
   <si>
-    <t>10. Person responding?</t>
-  </si>
-  <si>
     <t xml:space="preserve">11. Have you ever heard of Onchocerciasis disease? </t>
   </si>
   <si>
@@ -550,9 +541,6 @@
     <t>16.Did you swallow the MECTIZAN in front of the person who gave them to you?</t>
   </si>
   <si>
-    <t>17. Why did you swallow the MECTIZAN?</t>
-  </si>
-  <si>
     <t>18. Did you feel any side effects after swallowing the MECTIZAN?</t>
   </si>
   <si>
@@ -583,15 +571,9 @@
     <t>27. Do you have any suggestions to improve the communication around the MDA?</t>
   </si>
   <si>
-    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes'</t>
-  </si>
-  <si>
     <t>p_received_ivm</t>
   </si>
   <si>
-    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_received_ivm} = 'No'</t>
-  </si>
-  <si>
     <t>1=Absent</t>
   </si>
   <si>
@@ -658,9 +640,6 @@
     <t>${p_relationship_hhh} = 'Other'</t>
   </si>
   <si>
-    <t>${p_reason_not_received_ivm} = 'Other'</t>
-  </si>
-  <si>
     <t>p_swallow_ivm_in_front</t>
   </si>
   <si>
@@ -673,45 +652,15 @@
     <t>17. Specify the reason</t>
   </si>
   <si>
-    <t>${p_why_swallow_ivm} = 'Other'</t>
-  </si>
-  <si>
     <t>select_one why_swallow_ivm</t>
   </si>
   <si>
     <t>why_swallow_ivm</t>
   </si>
   <si>
-    <t>1=To be healthy</t>
-  </si>
-  <si>
-    <t>2=Afraid of getting the disease</t>
-  </si>
-  <si>
-    <t>3=Someone told me to</t>
-  </si>
-  <si>
-    <t>4=Everyone else is taking it</t>
-  </si>
-  <si>
-    <t>5=NA</t>
-  </si>
-  <si>
     <t>97=Other (specify)</t>
   </si>
   <si>
-    <t>To be healthy</t>
-  </si>
-  <si>
-    <t>Afraid of getting the disease</t>
-  </si>
-  <si>
-    <t>Someone told me to</t>
-  </si>
-  <si>
-    <t>Everyone else is taking it</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -778,9 +727,6 @@
     <t>p_received_alb</t>
   </si>
   <si>
-    <t>${p_reason_not_received_alb} = 'Other'</t>
-  </si>
-  <si>
     <t>p_swallow_alb</t>
   </si>
   <si>
@@ -835,9 +781,6 @@
     <t>p_were_in_village_trachoma</t>
   </si>
   <si>
-    <t>${p_consent} = 'Yes' and ${p_received_dk} = 'Yes'</t>
-  </si>
-  <si>
     <t xml:space="preserve">X0. Have you ever heard of Trachoma? </t>
   </si>
   <si>
@@ -871,9 +814,6 @@
     <t>p_reason_not_received_dk_other</t>
   </si>
   <si>
-    <t>${p_reason_not_received_dk} = 'Other'</t>
-  </si>
-  <si>
     <t>p_swallow_dk</t>
   </si>
   <si>
@@ -952,32 +892,141 @@
     <t>You just entered a value that will end the survey.</t>
   </si>
   <si>
-    <t>select_one responding</t>
-  </si>
-  <si>
     <t>p_reason_not_received_alb</t>
   </si>
   <si>
-    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_received_alb} = 'Yes'</t>
-  </si>
-  <si>
     <t>. &gt;= 0 and . &lt; 120</t>
   </si>
   <si>
     <t>Please enter a valide age</t>
   </si>
   <si>
-    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_swallow_ivm} = 'Yes'</t>
-  </si>
-  <si>
-    <t>(Sept 2023) SSD Cov ONCHO - 2.Formulaire Couverture</t>
+    <t xml:space="preserve">Correct month will be provided and please enumerator refer to the date provided. </t>
+  </si>
+  <si>
+    <t>17. Why didn't you swallow the MECTIZAN?</t>
+  </si>
+  <si>
+    <t>Sick</t>
+  </si>
+  <si>
+    <t>Breasthfeeding</t>
+  </si>
+  <si>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>4=Refused</t>
+  </si>
+  <si>
+    <t>3=Breathfeeding</t>
+  </si>
+  <si>
+    <t>2=Pregnant</t>
+  </si>
+  <si>
+    <t>1=Sick</t>
+  </si>
+  <si>
+    <t>(Sept 2023) SSD Cov ONCHO - 2.Formulaire Couverture V2</t>
+  </si>
+  <si>
+    <t>bf_oncho_cov_2_202309_couverture_v2</t>
+  </si>
+  <si>
+    <t>Lymphatic Filariasis</t>
+  </si>
+  <si>
+    <t>Onchocerciasis</t>
+  </si>
+  <si>
+    <t>Trachoma</t>
+  </si>
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>p_endelicity</t>
+  </si>
+  <si>
+    <t>Select the endemicity of the area</t>
+  </si>
+  <si>
+    <t>select_multiple disease</t>
+  </si>
+  <si>
+    <t>Lymphatic.Filariasis</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and selected(${p_endelicity}, 'Lymphatic.Filariasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_received_alb} = 'Yes' and selected(${p_endelicity}, 'Lymphatic.Filariasis')</t>
+  </si>
+  <si>
+    <t>${p_reason_not_received_alb} = 'Other' and selected(${p_endelicity}, 'Lymphatic.Filariasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and selected(${p_endelicity}, 'Lymphatic.Filariasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and selected(${p_endelicity}, 'Onchocerciasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and selected(${p_endelicity}, 'Onchocerciasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_received_ivm} = 'No' and selected(${p_endelicity}, 'Onchocerciasis')</t>
+  </si>
+  <si>
+    <t>${p_reason_not_received_ivm} = 'Other' and selected(${p_endelicity}, 'Onchocerciasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_swallow_ivm} = 'Yes' and selected(${p_endelicity}, 'Onchocerciasis')</t>
+  </si>
+  <si>
+    <r>
+      <t>${p_consent} = 'Yes' and ${p_were_in_village} = 'Yes' and ${p_swallow_ivm} = '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>No'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and selected(${p_endelicity}, 'Onchocerciasis')</t>
+    </r>
+  </si>
+  <si>
+    <t>${p_why_swallow_ivm} = 'Other' and selected(${p_endelicity}, 'Onchocerciasis')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and selected(${p_endelicity}, 'Trachoma')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_were_in_village_trachoma} = 'Yes' and selected(${p_endelicity}, 'Trachoma')</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_received_dk} = 'Yes' and selected(${p_endelicity}, 'Trachoma')</t>
+  </si>
+  <si>
+    <t>${p_reason_not_received_dk} = 'Other' and selected(${p_endelicity}, 'Trachoma')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1019,8 +1068,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,6 +1090,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1063,6 +1129,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,7 +1454,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1410,10 +1478,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1422,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -1442,22 +1510,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1465,10 +1533,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
@@ -1480,10 +1548,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
@@ -1495,10 +1563,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
@@ -1510,10 +1578,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
@@ -1525,20 +1593,20 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1546,305 +1614,301 @@
         <v>9</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="3"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>309</v>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>287</v>
+      </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>54</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
         <v>109</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>206</v>
+      <c r="H18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>135</v>
+      <c r="H21" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>305</v>
+        <v>132</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H22" t="s">
-        <v>110</v>
+      <c r="H22" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1852,81 +1916,83 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H24" t="s">
-        <v>110</v>
+      <c r="H24" s="3" t="s">
+        <v>311</v>
       </c>
       <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>288</v>
+      </c>
       <c r="E25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H25" t="s">
-        <v>110</v>
+      <c r="H25" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>182</v>
+        <v>312</v>
       </c>
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>184</v>
+        <v>313</v>
       </c>
       <c r="L27" s="13"/>
     </row>
@@ -1935,76 +2001,76 @@
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>207</v>
+        <v>314</v>
       </c>
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>182</v>
+        <v>312</v>
       </c>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>171</v>
+        <v>202</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>289</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="L31" s="13"/>
     </row>
@@ -2013,72 +2079,72 @@
         <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>212</v>
+        <v>317</v>
       </c>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>182</v>
+      <c r="H34" s="14" t="s">
+        <v>315</v>
       </c>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
@@ -2086,60 +2152,60 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H36" t="s">
-        <v>182</v>
+      <c r="H36" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H37" t="s">
-        <v>182</v>
+      <c r="H37" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2147,71 +2213,71 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>247</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>245</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H42" t="s">
-        <v>182</v>
+      <c r="H42" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2219,17 +2285,17 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H43" t="s">
-        <v>182</v>
+      <c r="H43" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2237,33 +2303,33 @@
         <v>9</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H44" t="s">
-        <v>110</v>
+      <c r="H44" s="3" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="10"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
@@ -2271,78 +2337,78 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H46" t="s">
-        <v>110</v>
+      <c r="H46" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H47" t="s">
-        <v>110</v>
+      <c r="H47" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H48" t="s">
-        <v>110</v>
+      <c r="H48" s="14" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>266</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2350,71 +2416,71 @@
         <v>9</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>278</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>266</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>266</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H53" t="s">
-        <v>110</v>
+      <c r="H53" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2422,19 +2488,19 @@
         <v>9</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H54" t="s">
-        <v>110</v>
+      <c r="H54" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2442,35 +2508,35 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H55" t="s">
-        <v>110</v>
+      <c r="H55" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
@@ -2478,110 +2544,110 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H57" t="s">
-        <v>110</v>
+      <c r="H57" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H58" t="s">
-        <v>110</v>
+      <c r="H58" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H59" t="s">
-        <v>110</v>
+      <c r="H59" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H60" t="s">
-        <v>110</v>
+      <c r="H60" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H61" t="s">
-        <v>110</v>
+      <c r="H61" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H62" t="s">
-        <v>110</v>
+      <c r="H62" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2593,13 +2659,13 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -2634,6 +2700,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2649,11 +2716,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2671,770 +2738,792 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" t="s">
         <v>123</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C31" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
         <v>142</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C40" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C42" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C43" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C45" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C46" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C48" t="s">
-        <v>215</v>
+        <v>290</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C49" t="s">
-        <v>216</v>
+        <v>137</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C50" t="s">
-        <v>217</v>
+        <v>291</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C51" t="s">
-        <v>218</v>
+        <v>292</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>225</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>214</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C53" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="C54" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="C56" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>225</v>
+        <v>274</v>
       </c>
       <c r="C57" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>294</v>
+        <v>238</v>
       </c>
       <c r="C58" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="C59" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>295</v>
+        <v>239</v>
       </c>
       <c r="C60" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="C61" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="C62" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>297</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>254</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>298</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>72</v>
+        <v>269</v>
       </c>
       <c r="C66" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="C67" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="C68" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>291</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>149</v>
+        <v>306</v>
       </c>
       <c r="C70" t="s">
-        <v>288</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C71" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C72" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -3456,13 +3545,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3478,10 +3567,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>298</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>21</v>

</xml_diff>